<commit_message>
Updated origin excel files
</commit_message>
<xml_diff>
--- a/endpoints/kettle/admin/quantitative_data/resources/origin/MM200.xlsx
+++ b/endpoints/kettle/admin/quantitative_data/resources/origin/MM200.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\ComEuropea\OSHA\OSHD15 - ESENER migration\03 - Data\Datos definitivos\ESENER 1\20150728_tables_OSHmanagement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\biserver-ce\pentaho-solutions\system\osha-dvt-esener\endpoints\kettle\admin\quantitative_data\resources\origin\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9120" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="MM200.1" sheetId="1" r:id="rId1"/>
@@ -179,25 +179,25 @@
     <t>EU27</t>
   </si>
   <si>
-    <t>MM200.1</t>
+    <t>MM200_1</t>
   </si>
   <si>
-    <t>MM200.2</t>
+    <t>MM200_2</t>
   </si>
   <si>
-    <t>MM200.3</t>
+    <t>MM200_3</t>
   </si>
   <si>
-    <t>MM200.4</t>
+    <t>MM200_4</t>
   </si>
   <si>
-    <t>MM200.5</t>
+    <t>MM200_5</t>
   </si>
   <si>
-    <t>MM200.6</t>
+    <t>MM200_6</t>
   </si>
   <si>
-    <t>MM200.7</t>
+    <t>MM200_7</t>
   </si>
 </sst>
 </file>
@@ -1023,21 +1023,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1059,6 +1044,42 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1074,18 +1095,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1100,15 +1109,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1399,7 +1399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K129"/>
   <sheetViews>
-    <sheetView topLeftCell="A112" workbookViewId="0">
+    <sheetView topLeftCell="A107" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:B124"/>
     </sheetView>
   </sheetViews>
@@ -5785,8 +5785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K129"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10196,7 +10196,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K129"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A104" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:B121"/>
     </sheetView>
   </sheetViews>
@@ -14507,7 +14507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K129"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
+    <sheetView topLeftCell="A109" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:B126"/>
     </sheetView>
   </sheetViews>
@@ -18943,8 +18943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K131"/>
   <sheetViews>
-    <sheetView topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="F116" sqref="F116"/>
+    <sheetView topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18952,18 +18952,18 @@
     <row r="1" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="148"/>
       <c r="C1" s="149"/>
-      <c r="D1" s="154" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="155"/>
-      <c r="F1" s="155"/>
-      <c r="G1" s="156"/>
-      <c r="H1" s="157" t="s">
+      <c r="D1" s="168" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="169"/>
+      <c r="F1" s="169"/>
+      <c r="G1" s="170"/>
+      <c r="H1" s="171" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="155"/>
-      <c r="J1" s="155"/>
-      <c r="K1" s="158"/>
+      <c r="I1" s="169"/>
+      <c r="J1" s="169"/>
+      <c r="K1" s="172"/>
     </row>
     <row r="2" spans="1:11" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="150" t="s">
@@ -23494,36 +23494,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K130"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="159"/>
-      <c r="C1" s="160"/>
-      <c r="D1" s="166" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="167"/>
-      <c r="F1" s="167"/>
-      <c r="G1" s="168"/>
-      <c r="H1" s="169" t="s">
+      <c r="A1" s="154"/>
+      <c r="C1" s="155"/>
+      <c r="D1" s="173" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="174"/>
+      <c r="F1" s="174"/>
+      <c r="G1" s="175"/>
+      <c r="H1" s="176" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="167"/>
-      <c r="J1" s="167"/>
-      <c r="K1" s="170"/>
+      <c r="I1" s="174"/>
+      <c r="J1" s="174"/>
+      <c r="K1" s="177"/>
     </row>
     <row r="2" spans="1:11" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="161" t="s">
+      <c r="A2" s="156" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="162" t="s">
+      <c r="C2" s="157" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="42" t="s">
@@ -23552,7 +23552,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="24.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="163" t="s">
+      <c r="A3" s="158" t="s">
         <v>17</v>
       </c>
       <c r="B3" t="s">
@@ -23587,7 +23587,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A4" s="164" t="s">
+      <c r="A4" s="159" t="s">
         <v>17</v>
       </c>
       <c r="B4" t="s">
@@ -23622,7 +23622,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A5" s="164" t="s">
+      <c r="A5" s="159" t="s">
         <v>17</v>
       </c>
       <c r="B5" t="s">
@@ -23657,7 +23657,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="164" t="s">
+      <c r="A6" s="159" t="s">
         <v>17</v>
       </c>
       <c r="B6" t="s">
@@ -23692,7 +23692,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="164" t="s">
+      <c r="A7" s="159" t="s">
         <v>18</v>
       </c>
       <c r="B7" t="s">
@@ -23727,7 +23727,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A8" s="164" t="s">
+      <c r="A8" s="159" t="s">
         <v>18</v>
       </c>
       <c r="B8" t="s">
@@ -23762,7 +23762,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A9" s="164" t="s">
+      <c r="A9" s="159" t="s">
         <v>18</v>
       </c>
       <c r="B9" t="s">
@@ -23797,7 +23797,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="164" t="s">
+      <c r="A10" s="159" t="s">
         <v>18</v>
       </c>
       <c r="B10" t="s">
@@ -23832,7 +23832,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="164" t="s">
+      <c r="A11" s="159" t="s">
         <v>19</v>
       </c>
       <c r="B11" t="s">
@@ -23867,7 +23867,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A12" s="164" t="s">
+      <c r="A12" s="159" t="s">
         <v>19</v>
       </c>
       <c r="B12" t="s">
@@ -23902,7 +23902,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A13" s="164" t="s">
+      <c r="A13" s="159" t="s">
         <v>19</v>
       </c>
       <c r="B13" t="s">
@@ -23937,7 +23937,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="164" t="s">
+      <c r="A14" s="159" t="s">
         <v>19</v>
       </c>
       <c r="B14" t="s">
@@ -23972,7 +23972,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="164" t="s">
+      <c r="A15" s="159" t="s">
         <v>20</v>
       </c>
       <c r="B15" t="s">
@@ -24007,7 +24007,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A16" s="164" t="s">
+      <c r="A16" s="159" t="s">
         <v>20</v>
       </c>
       <c r="B16" t="s">
@@ -24042,7 +24042,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A17" s="164" t="s">
+      <c r="A17" s="159" t="s">
         <v>20</v>
       </c>
       <c r="B17" t="s">
@@ -24077,7 +24077,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="164" t="s">
+      <c r="A18" s="159" t="s">
         <v>20</v>
       </c>
       <c r="B18" t="s">
@@ -24112,7 +24112,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="164" t="s">
+      <c r="A19" s="159" t="s">
         <v>21</v>
       </c>
       <c r="B19" t="s">
@@ -24147,7 +24147,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A20" s="164" t="s">
+      <c r="A20" s="159" t="s">
         <v>21</v>
       </c>
       <c r="B20" t="s">
@@ -24182,7 +24182,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A21" s="164" t="s">
+      <c r="A21" s="159" t="s">
         <v>21</v>
       </c>
       <c r="B21" t="s">
@@ -24217,7 +24217,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="164" t="s">
+      <c r="A22" s="159" t="s">
         <v>21</v>
       </c>
       <c r="B22" t="s">
@@ -24252,7 +24252,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="164" t="s">
+      <c r="A23" s="159" t="s">
         <v>22</v>
       </c>
       <c r="B23" t="s">
@@ -24287,7 +24287,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A24" s="164" t="s">
+      <c r="A24" s="159" t="s">
         <v>22</v>
       </c>
       <c r="B24" t="s">
@@ -24322,7 +24322,7 @@
       </c>
     </row>
     <row r="25" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A25" s="164" t="s">
+      <c r="A25" s="159" t="s">
         <v>22</v>
       </c>
       <c r="B25" t="s">
@@ -24357,7 +24357,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="164" t="s">
+      <c r="A26" s="159" t="s">
         <v>22</v>
       </c>
       <c r="B26" t="s">
@@ -24392,7 +24392,7 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="164" t="s">
+      <c r="A27" s="159" t="s">
         <v>23</v>
       </c>
       <c r="B27" t="s">
@@ -24427,7 +24427,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A28" s="164" t="s">
+      <c r="A28" s="159" t="s">
         <v>23</v>
       </c>
       <c r="B28" t="s">
@@ -24462,7 +24462,7 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A29" s="164" t="s">
+      <c r="A29" s="159" t="s">
         <v>23</v>
       </c>
       <c r="B29" t="s">
@@ -24497,7 +24497,7 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="164" t="s">
+      <c r="A30" s="159" t="s">
         <v>23</v>
       </c>
       <c r="B30" t="s">
@@ -24532,7 +24532,7 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="164" t="s">
+      <c r="A31" s="159" t="s">
         <v>24</v>
       </c>
       <c r="B31" t="s">
@@ -24567,7 +24567,7 @@
       </c>
     </row>
     <row r="32" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A32" s="164" t="s">
+      <c r="A32" s="159" t="s">
         <v>24</v>
       </c>
       <c r="B32" t="s">
@@ -24602,7 +24602,7 @@
       </c>
     </row>
     <row r="33" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A33" s="164" t="s">
+      <c r="A33" s="159" t="s">
         <v>24</v>
       </c>
       <c r="B33" t="s">
@@ -24637,7 +24637,7 @@
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="164" t="s">
+      <c r="A34" s="159" t="s">
         <v>24</v>
       </c>
       <c r="B34" t="s">
@@ -24672,7 +24672,7 @@
       </c>
     </row>
     <row r="35" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="164" t="s">
+      <c r="A35" s="159" t="s">
         <v>25</v>
       </c>
       <c r="B35" t="s">
@@ -24707,7 +24707,7 @@
       </c>
     </row>
     <row r="36" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A36" s="164" t="s">
+      <c r="A36" s="159" t="s">
         <v>25</v>
       </c>
       <c r="B36" t="s">
@@ -24742,7 +24742,7 @@
       </c>
     </row>
     <row r="37" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A37" s="164" t="s">
+      <c r="A37" s="159" t="s">
         <v>25</v>
       </c>
       <c r="B37" t="s">
@@ -24777,7 +24777,7 @@
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="164" t="s">
+      <c r="A38" s="159" t="s">
         <v>25</v>
       </c>
       <c r="B38" t="s">
@@ -24812,7 +24812,7 @@
       </c>
     </row>
     <row r="39" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="164" t="s">
+      <c r="A39" s="159" t="s">
         <v>26</v>
       </c>
       <c r="B39" t="s">
@@ -24847,7 +24847,7 @@
       </c>
     </row>
     <row r="40" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A40" s="164" t="s">
+      <c r="A40" s="159" t="s">
         <v>26</v>
       </c>
       <c r="B40" t="s">
@@ -24882,7 +24882,7 @@
       </c>
     </row>
     <row r="41" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A41" s="164" t="s">
+      <c r="A41" s="159" t="s">
         <v>26</v>
       </c>
       <c r="B41" t="s">
@@ -24917,7 +24917,7 @@
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="164" t="s">
+      <c r="A42" s="159" t="s">
         <v>26</v>
       </c>
       <c r="B42" t="s">
@@ -24952,7 +24952,7 @@
       </c>
     </row>
     <row r="43" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="164" t="s">
+      <c r="A43" s="159" t="s">
         <v>27</v>
       </c>
       <c r="B43" t="s">
@@ -24987,7 +24987,7 @@
       </c>
     </row>
     <row r="44" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A44" s="164" t="s">
+      <c r="A44" s="159" t="s">
         <v>27</v>
       </c>
       <c r="B44" t="s">
@@ -25022,7 +25022,7 @@
       </c>
     </row>
     <row r="45" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A45" s="164" t="s">
+      <c r="A45" s="159" t="s">
         <v>27</v>
       </c>
       <c r="B45" t="s">
@@ -25057,7 +25057,7 @@
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="164" t="s">
+      <c r="A46" s="159" t="s">
         <v>27</v>
       </c>
       <c r="B46" t="s">
@@ -25092,7 +25092,7 @@
       </c>
     </row>
     <row r="47" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="164" t="s">
+      <c r="A47" s="159" t="s">
         <v>28</v>
       </c>
       <c r="B47" t="s">
@@ -25127,7 +25127,7 @@
       </c>
     </row>
     <row r="48" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A48" s="164" t="s">
+      <c r="A48" s="159" t="s">
         <v>28</v>
       </c>
       <c r="B48" t="s">
@@ -25162,7 +25162,7 @@
       </c>
     </row>
     <row r="49" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A49" s="164" t="s">
+      <c r="A49" s="159" t="s">
         <v>28</v>
       </c>
       <c r="B49" t="s">
@@ -25197,7 +25197,7 @@
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="164" t="s">
+      <c r="A50" s="159" t="s">
         <v>28</v>
       </c>
       <c r="B50" t="s">
@@ -25232,7 +25232,7 @@
       </c>
     </row>
     <row r="51" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="164" t="s">
+      <c r="A51" s="159" t="s">
         <v>29</v>
       </c>
       <c r="B51" t="s">
@@ -25267,7 +25267,7 @@
       </c>
     </row>
     <row r="52" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A52" s="164" t="s">
+      <c r="A52" s="159" t="s">
         <v>29</v>
       </c>
       <c r="B52" t="s">
@@ -25302,7 +25302,7 @@
       </c>
     </row>
     <row r="53" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A53" s="164" t="s">
+      <c r="A53" s="159" t="s">
         <v>29</v>
       </c>
       <c r="B53" t="s">
@@ -25337,7 +25337,7 @@
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="164" t="s">
+      <c r="A54" s="159" t="s">
         <v>29</v>
       </c>
       <c r="B54" t="s">
@@ -25372,7 +25372,7 @@
       </c>
     </row>
     <row r="55" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="164" t="s">
+      <c r="A55" s="159" t="s">
         <v>30</v>
       </c>
       <c r="B55" t="s">
@@ -25407,7 +25407,7 @@
       </c>
     </row>
     <row r="56" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A56" s="164" t="s">
+      <c r="A56" s="159" t="s">
         <v>30</v>
       </c>
       <c r="B56" t="s">
@@ -25442,7 +25442,7 @@
       </c>
     </row>
     <row r="57" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A57" s="164" t="s">
+      <c r="A57" s="159" t="s">
         <v>30</v>
       </c>
       <c r="B57" t="s">
@@ -25477,7 +25477,7 @@
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="164" t="s">
+      <c r="A58" s="159" t="s">
         <v>30</v>
       </c>
       <c r="B58" t="s">
@@ -25512,7 +25512,7 @@
       </c>
     </row>
     <row r="59" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="164" t="s">
+      <c r="A59" s="159" t="s">
         <v>31</v>
       </c>
       <c r="B59" t="s">
@@ -25547,7 +25547,7 @@
       </c>
     </row>
     <row r="60" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A60" s="164" t="s">
+      <c r="A60" s="159" t="s">
         <v>31</v>
       </c>
       <c r="B60" t="s">
@@ -25582,7 +25582,7 @@
       </c>
     </row>
     <row r="61" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A61" s="164" t="s">
+      <c r="A61" s="159" t="s">
         <v>31</v>
       </c>
       <c r="B61" t="s">
@@ -25617,7 +25617,7 @@
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="164" t="s">
+      <c r="A62" s="159" t="s">
         <v>31</v>
       </c>
       <c r="B62" t="s">
@@ -25652,7 +25652,7 @@
       </c>
     </row>
     <row r="63" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="164" t="s">
+      <c r="A63" s="159" t="s">
         <v>32</v>
       </c>
       <c r="B63" t="s">
@@ -25687,7 +25687,7 @@
       </c>
     </row>
     <row r="64" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A64" s="164" t="s">
+      <c r="A64" s="159" t="s">
         <v>32</v>
       </c>
       <c r="B64" t="s">
@@ -25722,7 +25722,7 @@
       </c>
     </row>
     <row r="65" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A65" s="164" t="s">
+      <c r="A65" s="159" t="s">
         <v>32</v>
       </c>
       <c r="B65" t="s">
@@ -25757,7 +25757,7 @@
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A66" s="164" t="s">
+      <c r="A66" s="159" t="s">
         <v>32</v>
       </c>
       <c r="B66" t="s">
@@ -25792,7 +25792,7 @@
       </c>
     </row>
     <row r="67" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="164" t="s">
+      <c r="A67" s="159" t="s">
         <v>33</v>
       </c>
       <c r="B67" t="s">
@@ -25827,7 +25827,7 @@
       </c>
     </row>
     <row r="68" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A68" s="164" t="s">
+      <c r="A68" s="159" t="s">
         <v>33</v>
       </c>
       <c r="B68" t="s">
@@ -25862,7 +25862,7 @@
       </c>
     </row>
     <row r="69" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A69" s="164" t="s">
+      <c r="A69" s="159" t="s">
         <v>33</v>
       </c>
       <c r="B69" t="s">
@@ -25897,7 +25897,7 @@
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A70" s="164" t="s">
+      <c r="A70" s="159" t="s">
         <v>33</v>
       </c>
       <c r="B70" t="s">
@@ -25932,7 +25932,7 @@
       </c>
     </row>
     <row r="71" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="164" t="s">
+      <c r="A71" s="159" t="s">
         <v>34</v>
       </c>
       <c r="B71" t="s">
@@ -25967,7 +25967,7 @@
       </c>
     </row>
     <row r="72" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A72" s="164" t="s">
+      <c r="A72" s="159" t="s">
         <v>34</v>
       </c>
       <c r="B72" t="s">
@@ -26002,7 +26002,7 @@
       </c>
     </row>
     <row r="73" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A73" s="164" t="s">
+      <c r="A73" s="159" t="s">
         <v>34</v>
       </c>
       <c r="B73" t="s">
@@ -26037,7 +26037,7 @@
       </c>
     </row>
     <row r="74" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="164" t="s">
+      <c r="A74" s="159" t="s">
         <v>35</v>
       </c>
       <c r="B74" t="s">
@@ -26072,7 +26072,7 @@
       </c>
     </row>
     <row r="75" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A75" s="164" t="s">
+      <c r="A75" s="159" t="s">
         <v>35</v>
       </c>
       <c r="B75" t="s">
@@ -26107,7 +26107,7 @@
       </c>
     </row>
     <row r="76" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A76" s="164" t="s">
+      <c r="A76" s="159" t="s">
         <v>35</v>
       </c>
       <c r="B76" t="s">
@@ -26142,7 +26142,7 @@
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A77" s="164" t="s">
+      <c r="A77" s="159" t="s">
         <v>35</v>
       </c>
       <c r="B77" t="s">
@@ -26177,7 +26177,7 @@
       </c>
     </row>
     <row r="78" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="164" t="s">
+      <c r="A78" s="159" t="s">
         <v>36</v>
       </c>
       <c r="B78" t="s">
@@ -26212,7 +26212,7 @@
       </c>
     </row>
     <row r="79" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A79" s="164" t="s">
+      <c r="A79" s="159" t="s">
         <v>36</v>
       </c>
       <c r="B79" t="s">
@@ -26247,7 +26247,7 @@
       </c>
     </row>
     <row r="80" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A80" s="164" t="s">
+      <c r="A80" s="159" t="s">
         <v>36</v>
       </c>
       <c r="B80" t="s">
@@ -26282,7 +26282,7 @@
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A81" s="164" t="s">
+      <c r="A81" s="159" t="s">
         <v>36</v>
       </c>
       <c r="B81" t="s">
@@ -26317,7 +26317,7 @@
       </c>
     </row>
     <row r="82" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="164" t="s">
+      <c r="A82" s="159" t="s">
         <v>37</v>
       </c>
       <c r="B82" t="s">
@@ -26352,7 +26352,7 @@
       </c>
     </row>
     <row r="83" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A83" s="164" t="s">
+      <c r="A83" s="159" t="s">
         <v>37</v>
       </c>
       <c r="B83" t="s">
@@ -26387,7 +26387,7 @@
       </c>
     </row>
     <row r="84" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A84" s="164" t="s">
+      <c r="A84" s="159" t="s">
         <v>37</v>
       </c>
       <c r="B84" t="s">
@@ -26422,7 +26422,7 @@
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A85" s="164" t="s">
+      <c r="A85" s="159" t="s">
         <v>37</v>
       </c>
       <c r="B85" t="s">
@@ -26457,7 +26457,7 @@
       </c>
     </row>
     <row r="86" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="164" t="s">
+      <c r="A86" s="159" t="s">
         <v>38</v>
       </c>
       <c r="B86" t="s">
@@ -26492,7 +26492,7 @@
       </c>
     </row>
     <row r="87" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A87" s="164" t="s">
+      <c r="A87" s="159" t="s">
         <v>38</v>
       </c>
       <c r="B87" t="s">
@@ -26527,7 +26527,7 @@
       </c>
     </row>
     <row r="88" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A88" s="164" t="s">
+      <c r="A88" s="159" t="s">
         <v>38</v>
       </c>
       <c r="B88" t="s">
@@ -26562,7 +26562,7 @@
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A89" s="164" t="s">
+      <c r="A89" s="159" t="s">
         <v>38</v>
       </c>
       <c r="B89" t="s">
@@ -26597,7 +26597,7 @@
       </c>
     </row>
     <row r="90" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="164" t="s">
+      <c r="A90" s="159" t="s">
         <v>39</v>
       </c>
       <c r="B90" t="s">
@@ -26632,7 +26632,7 @@
       </c>
     </row>
     <row r="91" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A91" s="164" t="s">
+      <c r="A91" s="159" t="s">
         <v>39</v>
       </c>
       <c r="B91" t="s">
@@ -26667,7 +26667,7 @@
       </c>
     </row>
     <row r="92" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A92" s="164" t="s">
+      <c r="A92" s="159" t="s">
         <v>39</v>
       </c>
       <c r="B92" t="s">
@@ -26702,7 +26702,7 @@
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A93" s="164" t="s">
+      <c r="A93" s="159" t="s">
         <v>39</v>
       </c>
       <c r="B93" t="s">
@@ -26737,7 +26737,7 @@
       </c>
     </row>
     <row r="94" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="164" t="s">
+      <c r="A94" s="159" t="s">
         <v>40</v>
       </c>
       <c r="B94" t="s">
@@ -26772,7 +26772,7 @@
       </c>
     </row>
     <row r="95" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A95" s="164" t="s">
+      <c r="A95" s="159" t="s">
         <v>40</v>
       </c>
       <c r="B95" t="s">
@@ -26807,7 +26807,7 @@
       </c>
     </row>
     <row r="96" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A96" s="164" t="s">
+      <c r="A96" s="159" t="s">
         <v>40</v>
       </c>
       <c r="B96" t="s">
@@ -26842,7 +26842,7 @@
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A97" s="164" t="s">
+      <c r="A97" s="159" t="s">
         <v>40</v>
       </c>
       <c r="B97" t="s">
@@ -26877,7 +26877,7 @@
       </c>
     </row>
     <row r="98" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="164" t="s">
+      <c r="A98" s="159" t="s">
         <v>41</v>
       </c>
       <c r="B98" t="s">
@@ -26912,7 +26912,7 @@
       </c>
     </row>
     <row r="99" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A99" s="164" t="s">
+      <c r="A99" s="159" t="s">
         <v>41</v>
       </c>
       <c r="B99" t="s">
@@ -26947,7 +26947,7 @@
       </c>
     </row>
     <row r="100" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A100" s="164" t="s">
+      <c r="A100" s="159" t="s">
         <v>41</v>
       </c>
       <c r="B100" t="s">
@@ -26982,7 +26982,7 @@
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A101" s="164" t="s">
+      <c r="A101" s="159" t="s">
         <v>41</v>
       </c>
       <c r="B101" t="s">
@@ -27017,7 +27017,7 @@
       </c>
     </row>
     <row r="102" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="164" t="s">
+      <c r="A102" s="159" t="s">
         <v>42</v>
       </c>
       <c r="B102" t="s">
@@ -27052,7 +27052,7 @@
       </c>
     </row>
     <row r="103" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A103" s="164" t="s">
+      <c r="A103" s="159" t="s">
         <v>42</v>
       </c>
       <c r="B103" t="s">
@@ -27087,7 +27087,7 @@
       </c>
     </row>
     <row r="104" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A104" s="164" t="s">
+      <c r="A104" s="159" t="s">
         <v>42</v>
       </c>
       <c r="B104" t="s">
@@ -27122,7 +27122,7 @@
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A105" s="164" t="s">
+      <c r="A105" s="159" t="s">
         <v>42</v>
       </c>
       <c r="B105" t="s">
@@ -27157,7 +27157,7 @@
       </c>
     </row>
     <row r="106" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="164" t="s">
+      <c r="A106" s="159" t="s">
         <v>43</v>
       </c>
       <c r="B106" t="s">
@@ -27192,7 +27192,7 @@
       </c>
     </row>
     <row r="107" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A107" s="164" t="s">
+      <c r="A107" s="159" t="s">
         <v>43</v>
       </c>
       <c r="B107" t="s">
@@ -27227,7 +27227,7 @@
       </c>
     </row>
     <row r="108" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A108" s="164" t="s">
+      <c r="A108" s="159" t="s">
         <v>43</v>
       </c>
       <c r="B108" t="s">
@@ -27262,7 +27262,7 @@
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A109" s="164" t="s">
+      <c r="A109" s="159" t="s">
         <v>43</v>
       </c>
       <c r="B109" t="s">
@@ -27297,7 +27297,7 @@
       </c>
     </row>
     <row r="110" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="164" t="s">
+      <c r="A110" s="159" t="s">
         <v>44</v>
       </c>
       <c r="B110" t="s">
@@ -27332,7 +27332,7 @@
       </c>
     </row>
     <row r="111" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A111" s="164" t="s">
+      <c r="A111" s="159" t="s">
         <v>44</v>
       </c>
       <c r="B111" t="s">
@@ -27367,7 +27367,7 @@
       </c>
     </row>
     <row r="112" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A112" s="164" t="s">
+      <c r="A112" s="159" t="s">
         <v>44</v>
       </c>
       <c r="B112" t="s">
@@ -27402,7 +27402,7 @@
       </c>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A113" s="164" t="s">
+      <c r="A113" s="159" t="s">
         <v>44</v>
       </c>
       <c r="B113" t="s">
@@ -27437,7 +27437,7 @@
       </c>
     </row>
     <row r="114" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="164" t="s">
+      <c r="A114" s="159" t="s">
         <v>45</v>
       </c>
       <c r="B114" t="s">
@@ -27472,7 +27472,7 @@
       </c>
     </row>
     <row r="115" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A115" s="164" t="s">
+      <c r="A115" s="159" t="s">
         <v>45</v>
       </c>
       <c r="B115" t="s">
@@ -27507,7 +27507,7 @@
       </c>
     </row>
     <row r="116" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A116" s="164" t="s">
+      <c r="A116" s="159" t="s">
         <v>45</v>
       </c>
       <c r="B116" t="s">
@@ -27542,7 +27542,7 @@
       </c>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A117" s="164" t="s">
+      <c r="A117" s="159" t="s">
         <v>45</v>
       </c>
       <c r="B117" t="s">
@@ -27577,7 +27577,7 @@
       </c>
     </row>
     <row r="118" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="164" t="s">
+      <c r="A118" s="159" t="s">
         <v>46</v>
       </c>
       <c r="B118" t="s">
@@ -27612,7 +27612,7 @@
       </c>
     </row>
     <row r="119" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A119" s="164" t="s">
+      <c r="A119" s="159" t="s">
         <v>46</v>
       </c>
       <c r="B119" t="s">
@@ -27647,7 +27647,7 @@
       </c>
     </row>
     <row r="120" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A120" s="164" t="s">
+      <c r="A120" s="159" t="s">
         <v>46</v>
       </c>
       <c r="B120" t="s">
@@ -27682,7 +27682,7 @@
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A121" s="164" t="s">
+      <c r="A121" s="159" t="s">
         <v>46</v>
       </c>
       <c r="B121" t="s">
@@ -27717,7 +27717,7 @@
       </c>
     </row>
     <row r="122" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="164" t="s">
+      <c r="A122" s="159" t="s">
         <v>47</v>
       </c>
       <c r="B122" t="s">
@@ -27752,7 +27752,7 @@
       </c>
     </row>
     <row r="123" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A123" s="164" t="s">
+      <c r="A123" s="159" t="s">
         <v>47</v>
       </c>
       <c r="B123" t="s">
@@ -27787,7 +27787,7 @@
       </c>
     </row>
     <row r="124" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A124" s="164" t="s">
+      <c r="A124" s="159" t="s">
         <v>47</v>
       </c>
       <c r="B124" t="s">
@@ -27822,7 +27822,7 @@
       </c>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A125" s="164" t="s">
+      <c r="A125" s="159" t="s">
         <v>47</v>
       </c>
       <c r="B125" t="s">
@@ -27857,7 +27857,7 @@
       </c>
     </row>
     <row r="126" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="164" t="s">
+      <c r="A126" s="159" t="s">
         <v>48</v>
       </c>
       <c r="B126" t="s">
@@ -27892,7 +27892,7 @@
       </c>
     </row>
     <row r="127" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A127" s="164" t="s">
+      <c r="A127" s="159" t="s">
         <v>48</v>
       </c>
       <c r="B127" t="s">
@@ -27927,7 +27927,7 @@
       </c>
     </row>
     <row r="128" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A128" s="164" t="s">
+      <c r="A128" s="159" t="s">
         <v>48</v>
       </c>
       <c r="B128" t="s">
@@ -27962,7 +27962,7 @@
       </c>
     </row>
     <row r="129" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="165" t="s">
+      <c r="A129" s="160" t="s">
         <v>48</v>
       </c>
       <c r="B129" t="s">
@@ -28010,36 +28010,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="O109" sqref="O109"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="171"/>
-      <c r="C1" s="172"/>
-      <c r="D1" s="175" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="176"/>
-      <c r="F1" s="176"/>
-      <c r="G1" s="177"/>
-      <c r="H1" s="178" t="s">
+      <c r="A1" s="161"/>
+      <c r="C1" s="162"/>
+      <c r="D1" s="178" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="179"/>
+      <c r="F1" s="179"/>
+      <c r="G1" s="180"/>
+      <c r="H1" s="181" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="176"/>
-      <c r="J1" s="176"/>
-      <c r="K1" s="179"/>
+      <c r="I1" s="179"/>
+      <c r="J1" s="179"/>
+      <c r="K1" s="182"/>
     </row>
     <row r="2" spans="1:11" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="173" t="s">
+      <c r="A2" s="163" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="174" t="s">
+      <c r="C2" s="164" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="48" t="s">
@@ -28068,7 +28068,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="24.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="180" t="s">
+      <c r="A3" s="165" t="s">
         <v>17</v>
       </c>
       <c r="B3" t="s">
@@ -28103,7 +28103,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A4" s="181" t="s">
+      <c r="A4" s="166" t="s">
         <v>17</v>
       </c>
       <c r="B4" t="s">
@@ -28138,7 +28138,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A5" s="181" t="s">
+      <c r="A5" s="166" t="s">
         <v>17</v>
       </c>
       <c r="B5" t="s">
@@ -28173,7 +28173,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="181" t="s">
+      <c r="A6" s="166" t="s">
         <v>17</v>
       </c>
       <c r="B6" t="s">
@@ -28208,7 +28208,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="181" t="s">
+      <c r="A7" s="166" t="s">
         <v>18</v>
       </c>
       <c r="B7" t="s">
@@ -28243,7 +28243,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A8" s="181" t="s">
+      <c r="A8" s="166" t="s">
         <v>18</v>
       </c>
       <c r="B8" t="s">
@@ -28278,7 +28278,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A9" s="181" t="s">
+      <c r="A9" s="166" t="s">
         <v>18</v>
       </c>
       <c r="B9" t="s">
@@ -28313,7 +28313,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="181" t="s">
+      <c r="A10" s="166" t="s">
         <v>18</v>
       </c>
       <c r="B10" t="s">
@@ -28348,7 +28348,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="181" t="s">
+      <c r="A11" s="166" t="s">
         <v>19</v>
       </c>
       <c r="B11" t="s">
@@ -28383,7 +28383,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A12" s="181" t="s">
+      <c r="A12" s="166" t="s">
         <v>19</v>
       </c>
       <c r="B12" t="s">
@@ -28418,7 +28418,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A13" s="181" t="s">
+      <c r="A13" s="166" t="s">
         <v>19</v>
       </c>
       <c r="B13" t="s">
@@ -28453,7 +28453,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="181" t="s">
+      <c r="A14" s="166" t="s">
         <v>19</v>
       </c>
       <c r="B14" t="s">
@@ -28488,7 +28488,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="181" t="s">
+      <c r="A15" s="166" t="s">
         <v>20</v>
       </c>
       <c r="B15" t="s">
@@ -28523,7 +28523,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A16" s="181" t="s">
+      <c r="A16" s="166" t="s">
         <v>20</v>
       </c>
       <c r="B16" t="s">
@@ -28558,7 +28558,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A17" s="181" t="s">
+      <c r="A17" s="166" t="s">
         <v>20</v>
       </c>
       <c r="B17" t="s">
@@ -28593,7 +28593,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="181" t="s">
+      <c r="A18" s="166" t="s">
         <v>20</v>
       </c>
       <c r="B18" t="s">
@@ -28628,7 +28628,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="181" t="s">
+      <c r="A19" s="166" t="s">
         <v>21</v>
       </c>
       <c r="B19" t="s">
@@ -28663,7 +28663,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A20" s="181" t="s">
+      <c r="A20" s="166" t="s">
         <v>21</v>
       </c>
       <c r="B20" t="s">
@@ -28698,7 +28698,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A21" s="181" t="s">
+      <c r="A21" s="166" t="s">
         <v>21</v>
       </c>
       <c r="B21" t="s">
@@ -28733,7 +28733,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="181" t="s">
+      <c r="A22" s="166" t="s">
         <v>21</v>
       </c>
       <c r="B22" t="s">
@@ -28768,7 +28768,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="181" t="s">
+      <c r="A23" s="166" t="s">
         <v>22</v>
       </c>
       <c r="B23" t="s">
@@ -28803,7 +28803,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A24" s="181" t="s">
+      <c r="A24" s="166" t="s">
         <v>22</v>
       </c>
       <c r="B24" t="s">
@@ -28838,7 +28838,7 @@
       </c>
     </row>
     <row r="25" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A25" s="181" t="s">
+      <c r="A25" s="166" t="s">
         <v>22</v>
       </c>
       <c r="B25" t="s">
@@ -28873,7 +28873,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="181" t="s">
+      <c r="A26" s="166" t="s">
         <v>22</v>
       </c>
       <c r="B26" t="s">
@@ -28908,7 +28908,7 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="181" t="s">
+      <c r="A27" s="166" t="s">
         <v>23</v>
       </c>
       <c r="B27" t="s">
@@ -28943,7 +28943,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A28" s="181" t="s">
+      <c r="A28" s="166" t="s">
         <v>23</v>
       </c>
       <c r="B28" t="s">
@@ -28978,7 +28978,7 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A29" s="181" t="s">
+      <c r="A29" s="166" t="s">
         <v>23</v>
       </c>
       <c r="B29" t="s">
@@ -29013,7 +29013,7 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="181" t="s">
+      <c r="A30" s="166" t="s">
         <v>23</v>
       </c>
       <c r="B30" t="s">
@@ -29048,7 +29048,7 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="181" t="s">
+      <c r="A31" s="166" t="s">
         <v>24</v>
       </c>
       <c r="B31" t="s">
@@ -29083,7 +29083,7 @@
       </c>
     </row>
     <row r="32" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A32" s="181" t="s">
+      <c r="A32" s="166" t="s">
         <v>24</v>
       </c>
       <c r="B32" t="s">
@@ -29118,7 +29118,7 @@
       </c>
     </row>
     <row r="33" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A33" s="181" t="s">
+      <c r="A33" s="166" t="s">
         <v>24</v>
       </c>
       <c r="B33" t="s">
@@ -29153,7 +29153,7 @@
       </c>
     </row>
     <row r="34" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="181" t="s">
+      <c r="A34" s="166" t="s">
         <v>25</v>
       </c>
       <c r="B34" t="s">
@@ -29188,7 +29188,7 @@
       </c>
     </row>
     <row r="35" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A35" s="181" t="s">
+      <c r="A35" s="166" t="s">
         <v>25</v>
       </c>
       <c r="B35" t="s">
@@ -29223,7 +29223,7 @@
       </c>
     </row>
     <row r="36" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A36" s="181" t="s">
+      <c r="A36" s="166" t="s">
         <v>25</v>
       </c>
       <c r="B36" t="s">
@@ -29258,7 +29258,7 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="181" t="s">
+      <c r="A37" s="166" t="s">
         <v>25</v>
       </c>
       <c r="B37" t="s">
@@ -29293,7 +29293,7 @@
       </c>
     </row>
     <row r="38" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="181" t="s">
+      <c r="A38" s="166" t="s">
         <v>26</v>
       </c>
       <c r="B38" t="s">
@@ -29328,7 +29328,7 @@
       </c>
     </row>
     <row r="39" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A39" s="181" t="s">
+      <c r="A39" s="166" t="s">
         <v>26</v>
       </c>
       <c r="B39" t="s">
@@ -29363,7 +29363,7 @@
       </c>
     </row>
     <row r="40" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A40" s="181" t="s">
+      <c r="A40" s="166" t="s">
         <v>26</v>
       </c>
       <c r="B40" t="s">
@@ -29398,7 +29398,7 @@
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="181" t="s">
+      <c r="A41" s="166" t="s">
         <v>26</v>
       </c>
       <c r="B41" t="s">
@@ -29433,7 +29433,7 @@
       </c>
     </row>
     <row r="42" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="181" t="s">
+      <c r="A42" s="166" t="s">
         <v>27</v>
       </c>
       <c r="B42" t="s">
@@ -29468,7 +29468,7 @@
       </c>
     </row>
     <row r="43" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A43" s="181" t="s">
+      <c r="A43" s="166" t="s">
         <v>27</v>
       </c>
       <c r="B43" t="s">
@@ -29503,7 +29503,7 @@
       </c>
     </row>
     <row r="44" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A44" s="181" t="s">
+      <c r="A44" s="166" t="s">
         <v>27</v>
       </c>
       <c r="B44" t="s">
@@ -29538,7 +29538,7 @@
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="181" t="s">
+      <c r="A45" s="166" t="s">
         <v>27</v>
       </c>
       <c r="B45" t="s">
@@ -29573,7 +29573,7 @@
       </c>
     </row>
     <row r="46" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="181" t="s">
+      <c r="A46" s="166" t="s">
         <v>28</v>
       </c>
       <c r="B46" t="s">
@@ -29608,7 +29608,7 @@
       </c>
     </row>
     <row r="47" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A47" s="181" t="s">
+      <c r="A47" s="166" t="s">
         <v>28</v>
       </c>
       <c r="B47" t="s">
@@ -29643,7 +29643,7 @@
       </c>
     </row>
     <row r="48" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A48" s="181" t="s">
+      <c r="A48" s="166" t="s">
         <v>28</v>
       </c>
       <c r="B48" t="s">
@@ -29678,7 +29678,7 @@
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="181" t="s">
+      <c r="A49" s="166" t="s">
         <v>28</v>
       </c>
       <c r="B49" t="s">
@@ -29713,7 +29713,7 @@
       </c>
     </row>
     <row r="50" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="181" t="s">
+      <c r="A50" s="166" t="s">
         <v>29</v>
       </c>
       <c r="B50" t="s">
@@ -29748,7 +29748,7 @@
       </c>
     </row>
     <row r="51" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A51" s="181" t="s">
+      <c r="A51" s="166" t="s">
         <v>29</v>
       </c>
       <c r="B51" t="s">
@@ -29783,7 +29783,7 @@
       </c>
     </row>
     <row r="52" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A52" s="181" t="s">
+      <c r="A52" s="166" t="s">
         <v>29</v>
       </c>
       <c r="B52" t="s">
@@ -29818,7 +29818,7 @@
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="181" t="s">
+      <c r="A53" s="166" t="s">
         <v>29</v>
       </c>
       <c r="B53" t="s">
@@ -29853,7 +29853,7 @@
       </c>
     </row>
     <row r="54" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="181" t="s">
+      <c r="A54" s="166" t="s">
         <v>30</v>
       </c>
       <c r="B54" t="s">
@@ -29888,7 +29888,7 @@
       </c>
     </row>
     <row r="55" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A55" s="181" t="s">
+      <c r="A55" s="166" t="s">
         <v>30</v>
       </c>
       <c r="B55" t="s">
@@ -29923,7 +29923,7 @@
       </c>
     </row>
     <row r="56" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A56" s="181" t="s">
+      <c r="A56" s="166" t="s">
         <v>30</v>
       </c>
       <c r="B56" t="s">
@@ -29958,7 +29958,7 @@
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="181" t="s">
+      <c r="A57" s="166" t="s">
         <v>30</v>
       </c>
       <c r="B57" t="s">
@@ -29993,7 +29993,7 @@
       </c>
     </row>
     <row r="58" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="181" t="s">
+      <c r="A58" s="166" t="s">
         <v>31</v>
       </c>
       <c r="B58" t="s">
@@ -30028,7 +30028,7 @@
       </c>
     </row>
     <row r="59" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A59" s="181" t="s">
+      <c r="A59" s="166" t="s">
         <v>31</v>
       </c>
       <c r="B59" t="s">
@@ -30063,7 +30063,7 @@
       </c>
     </row>
     <row r="60" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A60" s="181" t="s">
+      <c r="A60" s="166" t="s">
         <v>31</v>
       </c>
       <c r="B60" t="s">
@@ -30098,7 +30098,7 @@
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" s="181" t="s">
+      <c r="A61" s="166" t="s">
         <v>31</v>
       </c>
       <c r="B61" t="s">
@@ -30133,7 +30133,7 @@
       </c>
     </row>
     <row r="62" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="181" t="s">
+      <c r="A62" s="166" t="s">
         <v>32</v>
       </c>
       <c r="B62" t="s">
@@ -30168,7 +30168,7 @@
       </c>
     </row>
     <row r="63" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A63" s="181" t="s">
+      <c r="A63" s="166" t="s">
         <v>32</v>
       </c>
       <c r="B63" t="s">
@@ -30203,7 +30203,7 @@
       </c>
     </row>
     <row r="64" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A64" s="181" t="s">
+      <c r="A64" s="166" t="s">
         <v>32</v>
       </c>
       <c r="B64" t="s">
@@ -30238,7 +30238,7 @@
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="181" t="s">
+      <c r="A65" s="166" t="s">
         <v>32</v>
       </c>
       <c r="B65" t="s">
@@ -30273,7 +30273,7 @@
       </c>
     </row>
     <row r="66" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="181" t="s">
+      <c r="A66" s="166" t="s">
         <v>33</v>
       </c>
       <c r="B66" t="s">
@@ -30308,7 +30308,7 @@
       </c>
     </row>
     <row r="67" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A67" s="181" t="s">
+      <c r="A67" s="166" t="s">
         <v>33</v>
       </c>
       <c r="B67" t="s">
@@ -30343,7 +30343,7 @@
       </c>
     </row>
     <row r="68" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A68" s="181" t="s">
+      <c r="A68" s="166" t="s">
         <v>33</v>
       </c>
       <c r="B68" t="s">
@@ -30378,7 +30378,7 @@
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A69" s="181" t="s">
+      <c r="A69" s="166" t="s">
         <v>33</v>
       </c>
       <c r="B69" t="s">
@@ -30413,7 +30413,7 @@
       </c>
     </row>
     <row r="70" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="181" t="s">
+      <c r="A70" s="166" t="s">
         <v>34</v>
       </c>
       <c r="B70" t="s">
@@ -30448,7 +30448,7 @@
       </c>
     </row>
     <row r="71" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A71" s="181" t="s">
+      <c r="A71" s="166" t="s">
         <v>34</v>
       </c>
       <c r="B71" t="s">
@@ -30483,7 +30483,7 @@
       </c>
     </row>
     <row r="72" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A72" s="181" t="s">
+      <c r="A72" s="166" t="s">
         <v>34</v>
       </c>
       <c r="B72" t="s">
@@ -30518,7 +30518,7 @@
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A73" s="181" t="s">
+      <c r="A73" s="166" t="s">
         <v>34</v>
       </c>
       <c r="B73" t="s">
@@ -30553,7 +30553,7 @@
       </c>
     </row>
     <row r="74" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="181" t="s">
+      <c r="A74" s="166" t="s">
         <v>35</v>
       </c>
       <c r="B74" t="s">
@@ -30588,7 +30588,7 @@
       </c>
     </row>
     <row r="75" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A75" s="181" t="s">
+      <c r="A75" s="166" t="s">
         <v>35</v>
       </c>
       <c r="B75" t="s">
@@ -30623,7 +30623,7 @@
       </c>
     </row>
     <row r="76" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A76" s="181" t="s">
+      <c r="A76" s="166" t="s">
         <v>35</v>
       </c>
       <c r="B76" t="s">
@@ -30658,7 +30658,7 @@
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A77" s="181" t="s">
+      <c r="A77" s="166" t="s">
         <v>35</v>
       </c>
       <c r="B77" t="s">
@@ -30693,7 +30693,7 @@
       </c>
     </row>
     <row r="78" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="181" t="s">
+      <c r="A78" s="166" t="s">
         <v>36</v>
       </c>
       <c r="B78" t="s">
@@ -30728,7 +30728,7 @@
       </c>
     </row>
     <row r="79" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A79" s="181" t="s">
+      <c r="A79" s="166" t="s">
         <v>36</v>
       </c>
       <c r="B79" t="s">
@@ -30763,7 +30763,7 @@
       </c>
     </row>
     <row r="80" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A80" s="181" t="s">
+      <c r="A80" s="166" t="s">
         <v>36</v>
       </c>
       <c r="B80" t="s">
@@ -30798,7 +30798,7 @@
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A81" s="181" t="s">
+      <c r="A81" s="166" t="s">
         <v>36</v>
       </c>
       <c r="B81" t="s">
@@ -30833,7 +30833,7 @@
       </c>
     </row>
     <row r="82" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="181" t="s">
+      <c r="A82" s="166" t="s">
         <v>37</v>
       </c>
       <c r="B82" t="s">
@@ -30868,7 +30868,7 @@
       </c>
     </row>
     <row r="83" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A83" s="181" t="s">
+      <c r="A83" s="166" t="s">
         <v>37</v>
       </c>
       <c r="B83" t="s">
@@ -30903,7 +30903,7 @@
       </c>
     </row>
     <row r="84" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A84" s="181" t="s">
+      <c r="A84" s="166" t="s">
         <v>37</v>
       </c>
       <c r="B84" t="s">
@@ -30938,7 +30938,7 @@
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A85" s="181" t="s">
+      <c r="A85" s="166" t="s">
         <v>37</v>
       </c>
       <c r="B85" t="s">
@@ -30973,7 +30973,7 @@
       </c>
     </row>
     <row r="86" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="181" t="s">
+      <c r="A86" s="166" t="s">
         <v>38</v>
       </c>
       <c r="B86" t="s">
@@ -31008,7 +31008,7 @@
       </c>
     </row>
     <row r="87" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A87" s="181" t="s">
+      <c r="A87" s="166" t="s">
         <v>38</v>
       </c>
       <c r="B87" t="s">
@@ -31043,7 +31043,7 @@
       </c>
     </row>
     <row r="88" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A88" s="181" t="s">
+      <c r="A88" s="166" t="s">
         <v>38</v>
       </c>
       <c r="B88" t="s">
@@ -31078,7 +31078,7 @@
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A89" s="181" t="s">
+      <c r="A89" s="166" t="s">
         <v>38</v>
       </c>
       <c r="B89" t="s">
@@ -31113,7 +31113,7 @@
       </c>
     </row>
     <row r="90" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="181" t="s">
+      <c r="A90" s="166" t="s">
         <v>39</v>
       </c>
       <c r="B90" t="s">
@@ -31148,7 +31148,7 @@
       </c>
     </row>
     <row r="91" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A91" s="181" t="s">
+      <c r="A91" s="166" t="s">
         <v>39</v>
       </c>
       <c r="B91" t="s">
@@ -31183,7 +31183,7 @@
       </c>
     </row>
     <row r="92" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A92" s="181" t="s">
+      <c r="A92" s="166" t="s">
         <v>39</v>
       </c>
       <c r="B92" t="s">
@@ -31218,7 +31218,7 @@
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A93" s="181" t="s">
+      <c r="A93" s="166" t="s">
         <v>39</v>
       </c>
       <c r="B93" t="s">
@@ -31253,7 +31253,7 @@
       </c>
     </row>
     <row r="94" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="181" t="s">
+      <c r="A94" s="166" t="s">
         <v>40</v>
       </c>
       <c r="B94" t="s">
@@ -31288,7 +31288,7 @@
       </c>
     </row>
     <row r="95" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A95" s="181" t="s">
+      <c r="A95" s="166" t="s">
         <v>40</v>
       </c>
       <c r="B95" t="s">
@@ -31323,7 +31323,7 @@
       </c>
     </row>
     <row r="96" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A96" s="181" t="s">
+      <c r="A96" s="166" t="s">
         <v>40</v>
       </c>
       <c r="B96" t="s">
@@ -31358,7 +31358,7 @@
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A97" s="181" t="s">
+      <c r="A97" s="166" t="s">
         <v>40</v>
       </c>
       <c r="B97" t="s">
@@ -31393,7 +31393,7 @@
       </c>
     </row>
     <row r="98" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="181" t="s">
+      <c r="A98" s="166" t="s">
         <v>41</v>
       </c>
       <c r="B98" t="s">
@@ -31428,7 +31428,7 @@
       </c>
     </row>
     <row r="99" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A99" s="181" t="s">
+      <c r="A99" s="166" t="s">
         <v>41</v>
       </c>
       <c r="B99" t="s">
@@ -31463,7 +31463,7 @@
       </c>
     </row>
     <row r="100" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A100" s="181" t="s">
+      <c r="A100" s="166" t="s">
         <v>41</v>
       </c>
       <c r="B100" t="s">
@@ -31498,7 +31498,7 @@
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A101" s="181" t="s">
+      <c r="A101" s="166" t="s">
         <v>41</v>
       </c>
       <c r="B101" t="s">
@@ -31533,7 +31533,7 @@
       </c>
     </row>
     <row r="102" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="181" t="s">
+      <c r="A102" s="166" t="s">
         <v>42</v>
       </c>
       <c r="B102" t="s">
@@ -31568,7 +31568,7 @@
       </c>
     </row>
     <row r="103" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A103" s="181" t="s">
+      <c r="A103" s="166" t="s">
         <v>42</v>
       </c>
       <c r="B103" t="s">
@@ -31603,7 +31603,7 @@
       </c>
     </row>
     <row r="104" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A104" s="181" t="s">
+      <c r="A104" s="166" t="s">
         <v>42</v>
       </c>
       <c r="B104" t="s">
@@ -31638,7 +31638,7 @@
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A105" s="181" t="s">
+      <c r="A105" s="166" t="s">
         <v>42</v>
       </c>
       <c r="B105" t="s">
@@ -31673,7 +31673,7 @@
       </c>
     </row>
     <row r="106" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="181" t="s">
+      <c r="A106" s="166" t="s">
         <v>43</v>
       </c>
       <c r="B106" t="s">
@@ -31708,7 +31708,7 @@
       </c>
     </row>
     <row r="107" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A107" s="181" t="s">
+      <c r="A107" s="166" t="s">
         <v>43</v>
       </c>
       <c r="B107" t="s">
@@ -31743,7 +31743,7 @@
       </c>
     </row>
     <row r="108" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A108" s="181" t="s">
+      <c r="A108" s="166" t="s">
         <v>43</v>
       </c>
       <c r="B108" t="s">
@@ -31778,7 +31778,7 @@
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A109" s="181" t="s">
+      <c r="A109" s="166" t="s">
         <v>43</v>
       </c>
       <c r="B109" t="s">
@@ -31813,7 +31813,7 @@
       </c>
     </row>
     <row r="110" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="181" t="s">
+      <c r="A110" s="166" t="s">
         <v>44</v>
       </c>
       <c r="B110" t="s">
@@ -31848,7 +31848,7 @@
       </c>
     </row>
     <row r="111" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A111" s="181" t="s">
+      <c r="A111" s="166" t="s">
         <v>44</v>
       </c>
       <c r="B111" t="s">
@@ -31883,7 +31883,7 @@
       </c>
     </row>
     <row r="112" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A112" s="181" t="s">
+      <c r="A112" s="166" t="s">
         <v>44</v>
       </c>
       <c r="B112" t="s">
@@ -31918,7 +31918,7 @@
       </c>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A113" s="181" t="s">
+      <c r="A113" s="166" t="s">
         <v>44</v>
       </c>
       <c r="B113" t="s">
@@ -31953,7 +31953,7 @@
       </c>
     </row>
     <row r="114" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="181" t="s">
+      <c r="A114" s="166" t="s">
         <v>45</v>
       </c>
       <c r="B114" t="s">
@@ -31988,7 +31988,7 @@
       </c>
     </row>
     <row r="115" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A115" s="181" t="s">
+      <c r="A115" s="166" t="s">
         <v>45</v>
       </c>
       <c r="B115" t="s">
@@ -32023,7 +32023,7 @@
       </c>
     </row>
     <row r="116" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A116" s="181" t="s">
+      <c r="A116" s="166" t="s">
         <v>45</v>
       </c>
       <c r="B116" t="s">
@@ -32058,7 +32058,7 @@
       </c>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A117" s="181" t="s">
+      <c r="A117" s="166" t="s">
         <v>45</v>
       </c>
       <c r="B117" t="s">
@@ -32093,7 +32093,7 @@
       </c>
     </row>
     <row r="118" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="181" t="s">
+      <c r="A118" s="166" t="s">
         <v>46</v>
       </c>
       <c r="B118" t="s">
@@ -32128,7 +32128,7 @@
       </c>
     </row>
     <row r="119" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A119" s="181" t="s">
+      <c r="A119" s="166" t="s">
         <v>46</v>
       </c>
       <c r="B119" t="s">
@@ -32163,7 +32163,7 @@
       </c>
     </row>
     <row r="120" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A120" s="181" t="s">
+      <c r="A120" s="166" t="s">
         <v>46</v>
       </c>
       <c r="B120" t="s">
@@ -32198,7 +32198,7 @@
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A121" s="181" t="s">
+      <c r="A121" s="166" t="s">
         <v>46</v>
       </c>
       <c r="B121" t="s">
@@ -32233,7 +32233,7 @@
       </c>
     </row>
     <row r="122" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="181" t="s">
+      <c r="A122" s="166" t="s">
         <v>47</v>
       </c>
       <c r="B122" t="s">
@@ -32268,7 +32268,7 @@
       </c>
     </row>
     <row r="123" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A123" s="181" t="s">
+      <c r="A123" s="166" t="s">
         <v>47</v>
       </c>
       <c r="B123" t="s">
@@ -32303,7 +32303,7 @@
       </c>
     </row>
     <row r="124" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A124" s="181" t="s">
+      <c r="A124" s="166" t="s">
         <v>47</v>
       </c>
       <c r="B124" t="s">
@@ -32338,7 +32338,7 @@
       </c>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A125" s="181" t="s">
+      <c r="A125" s="166" t="s">
         <v>47</v>
       </c>
       <c r="B125" t="s">
@@ -32373,7 +32373,7 @@
       </c>
     </row>
     <row r="126" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="181" t="s">
+      <c r="A126" s="166" t="s">
         <v>48</v>
       </c>
       <c r="B126" t="s">
@@ -32408,7 +32408,7 @@
       </c>
     </row>
     <row r="127" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A127" s="181" t="s">
+      <c r="A127" s="166" t="s">
         <v>48</v>
       </c>
       <c r="B127" t="s">
@@ -32443,7 +32443,7 @@
       </c>
     </row>
     <row r="128" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A128" s="181" t="s">
+      <c r="A128" s="166" t="s">
         <v>48</v>
       </c>
       <c r="B128" t="s">
@@ -32478,7 +32478,7 @@
       </c>
     </row>
     <row r="129" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="182" t="s">
+      <c r="A129" s="167" t="s">
         <v>48</v>
       </c>
       <c r="B129" t="s">

</xml_diff>